<commit_message>
Minor edits to program and emptying excel entries
</commit_message>
<xml_diff>
--- a/List.xlsx
+++ b/List.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Meeting password(leave blank if no</t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>Meeting ID(leave blank if not applicable</t>
-  </si>
-  <si>
-    <t>https://us04web.zoom.us/j/530059208?pwd=WEpNdCttYkVyNWN4dUowaFJnVzkwdz09</t>
   </si>
 </sst>
 </file>
@@ -372,7 +369,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,18 +396,11 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>43932.839583333334</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
+      <c r="A2" s="1"/>
+      <c r="B2" s="3"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>